<commit_message>
Update Week 11 - Financial Instruments.xlsx
</commit_message>
<xml_diff>
--- a/Advanced Corporate Reporting/Week 11 - Financial Instruments.xlsx
+++ b/Advanced Corporate Reporting/Week 11 - Financial Instruments.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\University-Resources\Advanced Corporate Reporting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D743D7E9-0F79-4413-AA42-682DC18A5C7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{A808E3F0-B683-4917-A1A8-6FC58A60415E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="21780" yWindow="4755" windowWidth="12345" windowHeight="12390" activeTab="1" xr2:uid="{9377C72A-D6F7-4967-A2F6-94A69B620D0C}"/>
+    <workbookView xWindow="19245" yWindow="4755" windowWidth="18900" windowHeight="12390" activeTab="1" xr2:uid="{9377C72A-D6F7-4967-A2F6-94A69B620D0C}"/>
   </bookViews>
   <sheets>
     <sheet name="Tutorial Questions" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
+    <sheet name="Lecture Notese" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="118">
   <si>
     <t>Oak plc issues 4% loan notes with a nominal value of £ 40,000. The loan notes are</t>
   </si>
@@ -373,12 +373,182 @@
   <si>
     <t>Year 5</t>
   </si>
+  <si>
+    <t>Understanding Compound Financial Instruments (IAS 32)</t>
+  </si>
+  <si>
+    <t>Key Principles:</t>
+  </si>
+  <si>
+    <t>Definition:</t>
+  </si>
+  <si>
+    <t>IAS 32 is pivotal in distinguishing between the liability and equity</t>
+  </si>
+  <si>
+    <t>components of compound financial instruments. A classic example</t>
+  </si>
+  <si>
+    <t>of such an instrument is a convertible bond. These bonds when issued</t>
+  </si>
+  <si>
+    <t>embed both a debt obligation and an option for the bondholder to</t>
+  </si>
+  <si>
+    <t>convert them into equity shares of the issuing company.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">components. The liability portion represents the issuer's obligation to </t>
+  </si>
+  <si>
+    <t>repay the debt, while the equity portion reflects its value.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">- </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Separation of Components</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: The core principle is the separation of these</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Measurement of Liability Component:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> The fair value of the liability</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">component is determined by discounting the future cash flows associated </t>
+  </si>
+  <si>
+    <t>with the debt. This involves estimating the interest payments and the principal</t>
+  </si>
+  <si>
+    <t>repayment, and then discounting these cash flows to their present value using</t>
+  </si>
+  <si>
+    <t>a market-related discount rate.</t>
+  </si>
+  <si>
+    <r>
+      <t>Derivation of Equity Component:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> The equity component's fair value</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> is not </t>
+    </r>
+  </si>
+  <si>
+    <t>directly measured. Instead, it's derived as the balancing figure. This means</t>
+  </si>
+  <si>
+    <t xml:space="preserve">it's the difference between the total proceeds received from issuing the instrument </t>
+  </si>
+  <si>
+    <t>and the fair value of the liability component.</t>
+  </si>
+  <si>
+    <t>Example Breakdown:</t>
+  </si>
+  <si>
+    <t>Let's dissect the provided example to illustrate these principles:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PV of Final Redemption (£13.5m * 0.567) </t>
+  </si>
+  <si>
+    <t>PV of Annual Interest (£10m * 4% * 3.605)</t>
+  </si>
+  <si>
+    <t>Liability Component (FV)</t>
+  </si>
+  <si>
+    <t>£'000</t>
+  </si>
+  <si>
+    <t>Total Instrument</t>
+  </si>
+  <si>
+    <t>Equity Component</t>
+  </si>
+  <si>
+    <t>Finance Charge (12%)</t>
+  </si>
+  <si>
+    <t>Annual Payment (4%)</t>
+  </si>
+  <si>
+    <t>Equity</t>
+  </si>
+  <si>
+    <t>SPL</t>
+  </si>
+  <si>
+    <t>Statement of Financial Position</t>
+  </si>
+  <si>
+    <t>Non-current liabilities:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Convertible debt </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Equity option </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Finance charge </t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
+    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="&quot;£&quot;#,##0.00"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
@@ -412,7 +582,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -420,16 +590,156 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -445,6 +755,67 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>19049</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>33025</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>643840</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{99F1BF6F-1411-5EE6-9CF4-7ADFE1F45466}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{BEBA8EAE-BF5A-486C-A8C5-ECC9F3942E4B}">
+              <a14:imgProps xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+                <a14:imgLayer r:embed="rId2">
+                  <a14:imgEffect>
+                    <a14:brightnessContrast bright="-44000" contrast="100000"/>
+                  </a14:imgEffect>
+                </a14:imgLayer>
+              </a14:imgProps>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6115049" y="985525"/>
+          <a:ext cx="4796741" cy="2100575"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -766,8 +1137,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10F259CA-A423-441D-80F2-641AD3BA3911}">
   <dimension ref="B2:K70"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="D71" sqref="D71"/>
+    <sheetView topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="B66" sqref="B66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1233,15 +1604,383 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE596340-4F92-461A-B523-F0E5A941C506}">
-  <dimension ref="A1"/>
+  <dimension ref="B2:Q45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="C40" sqref="C40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="12" max="12" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.5703125" customWidth="1"/>
+    <col min="16" max="17" width="11.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B2" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="3" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B3" s="5"/>
+    </row>
+    <row r="4" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B4" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="K4" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>84</v>
+      </c>
+      <c r="K5" s="6"/>
+    </row>
+    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B6" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="K6" s="8"/>
+    </row>
+    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>86</v>
+      </c>
+      <c r="K7" s="8"/>
+    </row>
+    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B8" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="K8" s="8"/>
+    </row>
+    <row r="9" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>88</v>
+      </c>
+      <c r="K9" s="8"/>
+    </row>
+    <row r="11" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B11" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="12" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B12" s="7" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="13" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="14" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="16" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B16" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="17" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="18" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>94</v>
+      </c>
+      <c r="P18" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="19" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>95</v>
+      </c>
+      <c r="K19" t="s">
+        <v>103</v>
+      </c>
+      <c r="P19" s="9">
+        <f>13500*0.567</f>
+        <v>7654.4999999999991</v>
+      </c>
+    </row>
+    <row r="20" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>96</v>
+      </c>
+      <c r="K20" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="L20" s="10"/>
+      <c r="M20" s="10"/>
+      <c r="N20" s="10"/>
+      <c r="P20" s="11">
+        <f>10000*0.04*3.605</f>
+        <v>1442</v>
+      </c>
+    </row>
+    <row r="21" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="K21" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="L21" s="1"/>
+      <c r="P21" s="26">
+        <f>P20+P19</f>
+        <v>9096.5</v>
+      </c>
+    </row>
+    <row r="22" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B22" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="P22" s="9"/>
+    </row>
+    <row r="23" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>98</v>
+      </c>
+      <c r="K23" t="s">
+        <v>107</v>
+      </c>
+      <c r="P23" s="9">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="24" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>99</v>
+      </c>
+      <c r="K24" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="L24" s="10"/>
+      <c r="M24" s="10"/>
+      <c r="P24" s="11">
+        <f>P21</f>
+        <v>9096.5</v>
+      </c>
+    </row>
+    <row r="25" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>100</v>
+      </c>
+      <c r="K25" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="L25" s="1"/>
+      <c r="P25" s="26">
+        <f>P23-P24</f>
+        <v>903.5</v>
+      </c>
+    </row>
+    <row r="27" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="28" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K28" s="18" t="s">
+        <v>71</v>
+      </c>
+      <c r="L28" s="19" t="s">
+        <v>72</v>
+      </c>
+      <c r="M28" s="19" t="s">
+        <v>109</v>
+      </c>
+      <c r="N28" s="19"/>
+      <c r="O28" s="19" t="s">
+        <v>110</v>
+      </c>
+      <c r="P28" s="19"/>
+      <c r="Q28" s="20" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="29" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="K29" s="16">
+        <v>2019</v>
+      </c>
+      <c r="L29" s="12">
+        <f>P21</f>
+        <v>9096.5</v>
+      </c>
+      <c r="M29" s="23">
+        <f>(12/100)*L29</f>
+        <v>1091.58</v>
+      </c>
+      <c r="N29" s="23"/>
+      <c r="O29" s="21">
+        <f>(4/100)*10000</f>
+        <v>400</v>
+      </c>
+      <c r="P29" s="21"/>
+      <c r="Q29" s="13">
+        <f>L29+M29-O29</f>
+        <v>9788.08</v>
+      </c>
+    </row>
+    <row r="30" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="K30" s="16">
+        <v>2020</v>
+      </c>
+      <c r="L30" s="12">
+        <f>Q29</f>
+        <v>9788.08</v>
+      </c>
+      <c r="M30" s="24">
+        <f t="shared" ref="M30:M33" si="0">(12/100)*L30</f>
+        <v>1174.5696</v>
+      </c>
+      <c r="N30" s="24"/>
+      <c r="O30" s="21">
+        <f t="shared" ref="O30:O33" si="1">(4/100)*10000</f>
+        <v>400</v>
+      </c>
+      <c r="P30" s="21"/>
+      <c r="Q30" s="13">
+        <f t="shared" ref="Q30:Q33" si="2">L30+M30-O30</f>
+        <v>10562.649600000001</v>
+      </c>
+    </row>
+    <row r="31" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="K31" s="16">
+        <v>2021</v>
+      </c>
+      <c r="L31" s="12">
+        <f>Q30</f>
+        <v>10562.649600000001</v>
+      </c>
+      <c r="M31" s="24">
+        <f t="shared" si="0"/>
+        <v>1267.5179519999999</v>
+      </c>
+      <c r="N31" s="24"/>
+      <c r="O31" s="21">
+        <f t="shared" si="1"/>
+        <v>400</v>
+      </c>
+      <c r="P31" s="21"/>
+      <c r="Q31" s="13">
+        <f t="shared" si="2"/>
+        <v>11430.167552000001</v>
+      </c>
+    </row>
+    <row r="32" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="K32" s="16">
+        <v>2022</v>
+      </c>
+      <c r="L32" s="12">
+        <f>Q31</f>
+        <v>11430.167552000001</v>
+      </c>
+      <c r="M32" s="24">
+        <f t="shared" si="0"/>
+        <v>1371.62010624</v>
+      </c>
+      <c r="N32" s="24"/>
+      <c r="O32" s="21">
+        <f t="shared" si="1"/>
+        <v>400</v>
+      </c>
+      <c r="P32" s="21"/>
+      <c r="Q32" s="13">
+        <f t="shared" si="2"/>
+        <v>12401.78765824</v>
+      </c>
+    </row>
+    <row r="33" spans="11:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K33" s="17">
+        <v>2023</v>
+      </c>
+      <c r="L33" s="14">
+        <f t="shared" ref="L31:L33" si="3">Q32</f>
+        <v>12401.78765824</v>
+      </c>
+      <c r="M33" s="25">
+        <f t="shared" si="0"/>
+        <v>1488.2145189887999</v>
+      </c>
+      <c r="N33" s="25"/>
+      <c r="O33" s="22">
+        <f t="shared" si="1"/>
+        <v>400</v>
+      </c>
+      <c r="P33" s="22"/>
+      <c r="Q33" s="15">
+        <f t="shared" si="2"/>
+        <v>13490.0021772288</v>
+      </c>
+    </row>
+    <row r="36" spans="11:17" x14ac:dyDescent="0.25">
+      <c r="K36" s="1" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="38" spans="11:17" x14ac:dyDescent="0.25">
+      <c r="K38" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="39" spans="11:17" x14ac:dyDescent="0.25">
+      <c r="K39" t="s">
+        <v>115</v>
+      </c>
+      <c r="M39" s="4">
+        <v>9788</v>
+      </c>
+    </row>
+    <row r="41" spans="11:17" x14ac:dyDescent="0.25">
+      <c r="K41" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="42" spans="11:17" x14ac:dyDescent="0.25">
+      <c r="K42" t="s">
+        <v>116</v>
+      </c>
+      <c r="M42">
+        <v>903.5</v>
+      </c>
+    </row>
+    <row r="44" spans="11:17" x14ac:dyDescent="0.25">
+      <c r="K44" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="45" spans="11:17" x14ac:dyDescent="0.25">
+      <c r="K45" t="s">
+        <v>117</v>
+      </c>
+      <c r="M45" s="4">
+        <v>1092</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="10">
+    <mergeCell ref="M29:N29"/>
+    <mergeCell ref="M30:N30"/>
+    <mergeCell ref="M31:N31"/>
+    <mergeCell ref="M32:N32"/>
+    <mergeCell ref="M33:N33"/>
+    <mergeCell ref="O29:P29"/>
+    <mergeCell ref="O30:P30"/>
+    <mergeCell ref="O31:P31"/>
+    <mergeCell ref="O33:P33"/>
+    <mergeCell ref="O32:P32"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -1503,14 +2242,14 @@
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AF8D09C3-901A-4B4E-9B15-2C08D6FF588B}">
   <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="fc68bb02-cea7-47a7-8486-5fa5775c5400"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="9ad45b7a-dbde-452b-a4a7-7cb6f25a272a"/>
-    <ds:schemaRef ds:uri="fc68bb02-cea7-47a7-8486-5fa5775c5400"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>

</xml_diff>